<commit_message>
Update structure of load_data and its testing
- The name of the file first_functions changed to load_data.R, from both R and test files.

- Update of test data and the tests
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/Dades prova.xlsx
+++ b/tests/testthat/test_data/Dades prova.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>municipi</t>
   </si>
@@ -52,6 +53,15 @@
   </si>
   <si>
     <t xml:space="preserve">Barcelona </t>
+  </si>
+  <si>
+    <t>L'espunyola</t>
+  </si>
+  <si>
+    <t>Arenys de Mar</t>
+  </si>
+  <si>
+    <t>Alpans13</t>
   </si>
 </sst>
 </file>
@@ -371,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -460,4 +470,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>